<commit_message>
added genreation to RD orderbook
</commit_message>
<xml_diff>
--- a/NL_bus_input2.xlsx
+++ b/NL_bus_input2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461D1285-F580-44D0-B84A-90012FE1A619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E91A17-5AF1-448B-8219-D05CFB128079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="2" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" activeTab="6" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Info &amp; case description</t>
   </si>
@@ -889,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F09800-6293-4D04-974E-A2660D60FC26}">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -2307,10 +2307,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A915C1-4CB9-4DD7-B6E4-10F8FAF3EAA1}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R11" sqref="R11:S13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2326,7 +2326,7 @@
     <col min="9" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -2345,8 +2345,11 @@
       <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -2368,8 +2371,11 @@
       <c r="G2" s="3">
         <v>20000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2391,8 +2397,11 @@
       <c r="G3" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2414,8 +2423,11 @@
       <c r="G4" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2437,8 +2449,11 @@
       <c r="G5" s="3">
         <v>50000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2460,8 +2475,11 @@
       <c r="G6" s="3">
         <v>9000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2482,6 +2500,9 @@
       </c>
       <c r="G7" s="3">
         <v>9000</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>